<commit_message>
Implement collision and object list
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD2B445-0A94-4CD0-8EA0-46C4D6332C67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5065AB-E780-48FF-BEF9-8839F02449C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Status</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>HP, Event Add</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Halfway done</t>
   </si>
 </sst>
 </file>
@@ -382,7 +388,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,7 +414,9 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -417,7 +425,9 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
Fix black screen bug
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFC69AA-8991-4399-A97B-4E2AFABF72D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1E1B14-9780-481A-AC33-BCB70EB1620C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Status</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Improve Object Interaction</t>
+  </si>
+  <si>
+    <t>Improve Get Tile Image</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +530,15 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>

</xml_diff>